<commit_message>
Added tiles and plates, updated 70827 BOM
</commit_message>
<xml_diff>
--- a/BOM's/70827 Ultrakatty with Warrior Lucy - 300%.xlsx
+++ b/BOM's/70827 Ultrakatty with Warrior Lucy - 300%.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Håkan\OneDrive\Lego\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RepRap\_Git\LEGO\BOM's\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Black" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="88">
   <si>
     <t>Tile 2 x 2 Round</t>
   </si>
@@ -292,6 +292,15 @@
   </si>
   <si>
     <t>Act time</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Cut @ 7,8</t>
+  </si>
+  <si>
+    <t>45 deg support for groove</t>
   </si>
 </sst>
 </file>
@@ -339,10 +348,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -626,8 +636,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -685,6 +695,9 @@
       </c>
       <c r="G2" s="1">
         <v>2.4664351851851851E-2</v>
+      </c>
+      <c r="H2" s="1">
+        <v>2.7083333333333334E-2</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -1175,102 +1188,218 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="35.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="10.77734375" customWidth="1"/>
+    <col min="6" max="6" width="10.77734375" style="2" customWidth="1"/>
+    <col min="7" max="8" width="10.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="I1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2">
         <v>11458</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="C1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2">
+      <c r="C2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3">
         <v>2431</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>9</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>3.92</v>
+      </c>
+      <c r="E3">
+        <v>11.7</v>
+      </c>
+      <c r="F3" s="2">
+        <v>3.5</v>
+      </c>
+      <c r="G3" s="3">
+        <v>3.8495370370370367E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4">
         <v>3001</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>10</v>
       </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4">
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>28.92</v>
+      </c>
+      <c r="E4">
+        <v>86.24</v>
+      </c>
+      <c r="F4" s="2">
+        <v>25.79</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0.31452546296296297</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5">
         <v>3020</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>11</v>
       </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5">
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>7.65</v>
+      </c>
+      <c r="E5">
+        <v>22.81</v>
+      </c>
+      <c r="F5" s="2">
+        <v>6.82</v>
+      </c>
+      <c r="G5" s="3">
+        <v>7.0717592592592596E-2</v>
+      </c>
+      <c r="H5" s="3">
+        <v>7.1527777777777787E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6">
         <v>3031</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>12</v>
       </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6">
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>14.84</v>
+      </c>
+      <c r="E6">
+        <v>44.27</v>
+      </c>
+      <c r="F6" s="2">
+        <v>13.24</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0.13685185185185186</v>
+      </c>
+      <c r="H6" s="3">
+        <v>0.1388888888888889</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7">
         <v>6141</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>13</v>
       </c>
-      <c r="C6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7">
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>1.08</v>
+      </c>
+      <c r="E7">
+        <v>3.21</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0.96</v>
+      </c>
+      <c r="G7" s="3">
+        <v>1.4606481481481482E-2</v>
+      </c>
+      <c r="I7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8">
         <v>87580</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>14</v>
       </c>
-      <c r="C7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8">
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <v>3.98</v>
+      </c>
+      <c r="E8">
+        <v>11.6</v>
+      </c>
+      <c r="F8" s="2">
+        <v>3.47</v>
+      </c>
+      <c r="G8" s="3">
+        <v>3.8657407407407404E-2</v>
+      </c>
+      <c r="I8" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9">
         <v>98138</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>15</v>
       </c>
-      <c r="C8">
+      <c r="C9">
         <v>2</v>
       </c>
     </row>
@@ -1281,10 +1410,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1292,7 +1421,7 @@
     <col min="2" max="2" width="49" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>11477</v>
       </c>
@@ -1303,7 +1432,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>15209</v>
       </c>
@@ -1314,7 +1443,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>18677</v>
       </c>
@@ -1325,7 +1454,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>24201</v>
       </c>
@@ -1336,7 +1465,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2456</v>
       </c>
@@ -1346,8 +1475,20 @@
       <c r="C5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D5">
+        <v>21.43</v>
+      </c>
+      <c r="E5">
+        <v>64.42</v>
+      </c>
+      <c r="F5">
+        <v>19.260000000000002</v>
+      </c>
+      <c r="G5" s="3">
+        <v>0.23608796296296297</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>26601</v>
       </c>
@@ -1358,7 +1499,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>3005</v>
       </c>
@@ -1368,8 +1509,20 @@
       <c r="C7">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D7">
+        <v>4.93</v>
+      </c>
+      <c r="E7">
+        <v>14.81</v>
+      </c>
+      <c r="F7">
+        <v>4.43</v>
+      </c>
+      <c r="G7" s="3">
+        <v>5.950231481481482E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>3010</v>
       </c>
@@ -1379,8 +1532,20 @@
       <c r="C8">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D8">
+        <v>35.090000000000003</v>
+      </c>
+      <c r="E8">
+        <v>105.49</v>
+      </c>
+      <c r="F8">
+        <v>31.54</v>
+      </c>
+      <c r="G8" s="3">
+        <v>0.38418981481481485</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>3020</v>
       </c>
@@ -1390,8 +1555,20 @@
       <c r="C9">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D9">
+        <v>30.53</v>
+      </c>
+      <c r="E9">
+        <v>91.79</v>
+      </c>
+      <c r="F9">
+        <v>27.45</v>
+      </c>
+      <c r="G9" s="3">
+        <v>0.28556712962962966</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>3021</v>
       </c>
@@ -1401,8 +1578,20 @@
       <c r="C10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D10">
+        <v>5.8</v>
+      </c>
+      <c r="E10">
+        <v>17.43</v>
+      </c>
+      <c r="F10">
+        <v>5.21</v>
+      </c>
+      <c r="G10" s="3">
+        <v>5.451388888888889E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>3023</v>
       </c>
@@ -1412,8 +1601,20 @@
       <c r="C11">
         <v>6</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D11">
+        <v>13.22</v>
+      </c>
+      <c r="E11">
+        <v>39.74</v>
+      </c>
+      <c r="F11">
+        <v>11.88</v>
+      </c>
+      <c r="G11" s="3">
+        <v>0.13328703703703704</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>3024</v>
       </c>
@@ -1423,8 +1624,20 @@
       <c r="C12">
         <v>16</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D12">
+        <v>18.47</v>
+      </c>
+      <c r="E12">
+        <v>55.52</v>
+      </c>
+      <c r="F12">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="G12" s="3">
+        <v>0.19582175925925926</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>30383</v>
       </c>
@@ -1435,7 +1648,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>3623</v>
       </c>
@@ -1445,8 +1658,20 @@
       <c r="C14">
         <v>8</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D14">
+        <v>25.88</v>
+      </c>
+      <c r="E14">
+        <v>77.81</v>
+      </c>
+      <c r="F14">
+        <v>23.26</v>
+      </c>
+      <c r="G14" s="3">
+        <v>0.25655092592592593</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>44301</v>
       </c>
@@ -1457,7 +1682,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>44302</v>
       </c>
@@ -1600,26 +1825,68 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="28" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2">
         <v>30260</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
         <v>40</v>
       </c>
-      <c r="C1">
-        <v>1</v>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1.96</v>
+      </c>
+      <c r="E2">
+        <v>5.89</v>
+      </c>
+      <c r="F2" s="2">
+        <v>1.76</v>
+      </c>
+      <c r="G2" s="3">
+        <v>2.0879629629629626E-2</v>
+      </c>
+      <c r="H2" s="3">
+        <v>2.2222222222222223E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>